<commit_message>
HW169 Steering Wheel Interface rev3 - schmitt trigger fixes
* HW169 Steering Wheel Interface rev3
Overall
- Regenerated BOM
- Fixed lane assist connection to schmitt trigger
- Moved some labels on pcb for readability
</commit_message>
<xml_diff>
--- a/MSXII_SteeringWheelInterfaceBoard/Project Outputs for MSXII_SteeringWheelInterfaceBoard/MSXII_SteeringWheelInterfaceBoard_3.0.xlsx
+++ b/MSXII_SteeringWheelInterfaceBoard/Project Outputs for MSXII_SteeringWheelInterfaceBoard/MSXII_SteeringWheelInterfaceBoard_3.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jieni\Documents\Github\hardware\MSXII_SteeringWheelInterfaceBoard\Project Outputs for MSXII_SteeringWheelInterfaceBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4244F6A-DC50-450A-A771-9DD51F8BFA0B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{720FA082-38A0-43B1-A714-62F78AFEB73C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1837" yWindow="2438" windowWidth="15391" windowHeight="9532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1013" yWindow="1477" windowWidth="13027" windowHeight="9533" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="115">
   <si>
     <t>Title</t>
   </si>
@@ -108,6 +108,10 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>2019/4/3 下午 6:14</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>1</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -294,7 +298,7 @@
     <t>OPA2197IDGKR</t>
   </si>
   <si>
-    <t>M74HC14YTTR</t>
+    <t>M74HC14YRM13TR</t>
   </si>
   <si>
     <t>Supplier 1</t>
@@ -350,7 +354,7 @@
     <t>296-47349-1-ND</t>
   </si>
   <si>
-    <t>497-14387-1-ND</t>
+    <t>497-14386-1-ND</t>
   </si>
   <si>
     <t>Supplier Unit Price 1</t>
@@ -374,6 +378,10 @@
   </si>
   <si>
     <t>Bill of Materials for Project [MSXII_SteeringWheelInterfaceBoard.PrjPcb] (No PCB Document Selected)</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>下午 6:14</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
@@ -487,112 +495,102 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -976,602 +974,602 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.265625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="38.265625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="28.73046875" style="26" customWidth="1"/>
-    <col min="4" max="4" width="26.1328125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12" style="6" customWidth="1"/>
-    <col min="6" max="6" width="21" style="6" customWidth="1"/>
-    <col min="7" max="7" width="19.3984375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="16" style="6" customWidth="1"/>
-    <col min="9" max="9" width="20" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="6"/>
+    <col min="1" max="1" width="41.265625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="38.265625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="28.73046875" style="25" customWidth="1"/>
+    <col min="4" max="4" width="26.1328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12" style="5" customWidth="1"/>
+    <col min="6" max="6" width="21" style="5" customWidth="1"/>
+    <col min="7" max="7" width="19.3984375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="16" style="5" customWidth="1"/>
+    <col min="9" max="9" width="20" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="22">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.35">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="32">
-        <v>43530.705555555556</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="B6" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="27"/>
-      <c r="J7" s="8"/>
+      <c r="B7" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="27"/>
+      <c r="B8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="26"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="24">
         <v>55</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="26"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="27"/>
-    </row>
-    <row r="11" spans="1:10" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="22" t="s">
+      <c r="C10" s="26"/>
+    </row>
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.47971000000000003</v>
+      </c>
+      <c r="H12" s="2">
+        <v>8</v>
+      </c>
+      <c r="I12" s="9">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.15323999999999999</v>
+      </c>
+      <c r="H13" s="2">
+        <v>13</v>
+      </c>
+      <c r="I13" s="9">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.49303999999999998</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="9">
+        <v>0.49303999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.18654999999999999</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0.18654999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.87</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="9">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1722861302</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1.95</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.13325000000000001</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0.13325000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.46639000000000003</v>
+      </c>
+      <c r="H20" s="2">
+        <v>4</v>
+      </c>
+      <c r="I20" s="9">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3.1980000000000001E-2</v>
+      </c>
+      <c r="H21" s="2">
+        <v>10</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0.31980999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.13325000000000001</v>
+      </c>
+      <c r="H22" s="2">
+        <v>4</v>
+      </c>
+      <c r="I22" s="9">
+        <v>0.53300999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.13325000000000001</v>
+      </c>
+      <c r="H23" s="2">
+        <v>6</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0.79952000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.38643</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
+      <c r="I24" s="9">
+        <v>0.38643</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="2">
+        <v>3.21</v>
+      </c>
+      <c r="H25" s="2">
+        <v>2</v>
+      </c>
+      <c r="I25" s="9">
+        <v>6.42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="B26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="C26" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="D26" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="E26" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="F26" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="H11" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="I11" s="22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0.48385</v>
-      </c>
-      <c r="H12" s="3">
-        <v>8</v>
-      </c>
-      <c r="I12" s="10">
-        <v>3.87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.15456</v>
-      </c>
-      <c r="H13" s="3">
-        <v>13</v>
-      </c>
-      <c r="I13" s="10">
-        <v>2.0099999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.49729000000000001</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="G26" s="2">
+        <v>0.63961000000000001</v>
+      </c>
+      <c r="H26" s="2">
         <v>1</v>
       </c>
-      <c r="I14" s="10">
-        <v>0.49729000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0.18815999999999999</v>
-      </c>
-      <c r="H15" s="3">
-        <v>1</v>
-      </c>
-      <c r="I15" s="10">
-        <v>0.18815999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1.88</v>
-      </c>
-      <c r="H16" s="3">
-        <v>1</v>
-      </c>
-      <c r="I16" s="10">
-        <v>1.88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" s="3">
-        <v>1.05</v>
-      </c>
-      <c r="H17" s="3">
-        <v>1</v>
-      </c>
-      <c r="I17" s="10">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1722861302</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G18" s="3">
-        <v>1.96</v>
-      </c>
-      <c r="H18" s="3">
-        <v>1</v>
-      </c>
-      <c r="I18" s="10">
-        <v>1.96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.13439999999999999</v>
-      </c>
-      <c r="H19" s="3">
-        <v>1</v>
-      </c>
-      <c r="I19" s="10">
-        <v>0.13439999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0.47040999999999999</v>
-      </c>
-      <c r="H20" s="3">
-        <v>4</v>
-      </c>
-      <c r="I20" s="10">
-        <v>1.88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="G21" s="3">
-        <v>3.2259999999999997E-2</v>
-      </c>
-      <c r="H21" s="3">
-        <v>10</v>
-      </c>
-      <c r="I21" s="10">
-        <v>0.32257000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0.13439999999999999</v>
-      </c>
-      <c r="H22" s="3">
-        <v>4</v>
-      </c>
-      <c r="I22" s="10">
-        <v>0.53761000000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="3">
-        <v>0.13439999999999999</v>
-      </c>
-      <c r="H23" s="3">
-        <v>6</v>
-      </c>
-      <c r="I23" s="10">
-        <v>0.80642000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0.38977000000000001</v>
-      </c>
-      <c r="H24" s="3">
-        <v>1</v>
-      </c>
-      <c r="I24" s="10">
-        <v>0.38977000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G25" s="3">
-        <v>3.24</v>
-      </c>
-      <c r="H25" s="3">
-        <v>2</v>
-      </c>
-      <c r="I25" s="10">
-        <v>6.48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="G26" s="3">
-        <v>0.59136999999999995</v>
-      </c>
-      <c r="H26" s="3">
-        <v>1</v>
-      </c>
-      <c r="I26" s="10">
-        <v>0.59136999999999995</v>
+      <c r="I26" s="9">
+        <v>0.63961000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="3" t="s">
+      <c r="A27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I27" s="14">
+      <c r="I27" s="13">
         <f>SUM(I12:I26)</f>
-        <v>22.597590000000004</v>
+        <v>22.471220000000002</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="17"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="16"/>
     </row>
     <row r="29" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="17"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1597,121 +1595,120 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.265625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="108.59765625" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="30.265625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="108.59765625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="B1" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
+      <c r="B6" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="20">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="33">
-        <v>0.7055555555555556</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+      <c r="B8" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="34">
-        <v>43530</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+      <c r="B9" s="31">
+        <v>43558</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="35">
-        <v>43530.705555555556</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="B10" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
+      <c r="B11" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20" t="s">
+      <c r="B12" s="20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>